<commit_message>
New R Visualisations surrounding pie charts and scatter plots
</commit_message>
<xml_diff>
--- a/Matlab/V.xlsx
+++ b/Matlab/V.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cathe\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D2C1E36-548C-46FA-B1E2-C06C7D6367A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45F5F12A-3E3C-478E-BBD4-6DDD719B7DA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1884" yWindow="696" windowWidth="17280" windowHeight="11664" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="22">
   <si>
     <t>vs.</t>
   </si>
@@ -91,7 +91,7 @@
     <t>Stem</t>
   </si>
   <si>
-    <t>Heatmap</t>
+    <t>Bubble</t>
   </si>
 </sst>
 </file>
@@ -107,7 +107,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -117,12 +117,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -139,13 +133,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -428,8 +421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40:XFD40"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -911,7 +904,7 @@
   <dimension ref="A1:L121"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="A63" sqref="A63:XFD63"/>
+      <selection activeCell="K70" sqref="K70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1003,6 +996,13 @@
       <c r="E5" t="s">
         <v>8</v>
       </c>
+      <c r="J5" s="2"/>
+      <c r="K5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L5" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -1655,9 +1655,9 @@
       <c r="E63" t="s">
         <v>11</v>
       </c>
-      <c r="J63" s="3"/>
+      <c r="J63" s="2"/>
       <c r="K63" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="L63" t="s">
         <v>14</v>
@@ -1672,6 +1672,13 @@
       </c>
       <c r="E64" t="s">
         <v>12</v>
+      </c>
+      <c r="J64" s="2"/>
+      <c r="K64" t="s">
+        <v>19</v>
+      </c>
+      <c r="L64" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>